<commit_message>
Mejoras en graficas y excel
</commit_message>
<xml_diff>
--- a/GRAFICAS/estadisticas.xlsx
+++ b/GRAFICAS/estadisticas.xlsx
@@ -11,26 +11,27 @@
     <sheet name="dias_fiebre" sheetId="2" r:id="rId2"/>
     <sheet name="dias_ultima_fiebre" sheetId="3" r:id="rId3"/>
     <sheet name="nauseas" sheetId="4" r:id="rId4"/>
-    <sheet name="rash" sheetId="5" r:id="rId5"/>
-    <sheet name="vomitos" sheetId="6" r:id="rId6"/>
+    <sheet name="vomitos" sheetId="5" r:id="rId5"/>
+    <sheet name="rash" sheetId="6" r:id="rId6"/>
     <sheet name="mialgias" sheetId="7" r:id="rId7"/>
     <sheet name="artralgias" sheetId="8" r:id="rId8"/>
-    <sheet name="dolor_abdominal" sheetId="9" r:id="rId9"/>
-    <sheet name="acumulacion_fluidos" sheetId="10" r:id="rId10"/>
-    <sheet name="sangrado_mucosas" sheetId="11" r:id="rId11"/>
-    <sheet name="hemorragia" sheetId="12" r:id="rId12"/>
-    <sheet name="letargia" sheetId="13" r:id="rId13"/>
-    <sheet name="irritabilidad" sheetId="14" r:id="rId14"/>
-    <sheet name="shock" sheetId="15" r:id="rId15"/>
-    <sheet name="prueba_torniquete" sheetId="16" r:id="rId16"/>
+    <sheet name="prueba_torniquete" sheetId="9" r:id="rId9"/>
+    <sheet name="dolor_abdominal" sheetId="10" r:id="rId10"/>
+    <sheet name="acumulacion_fluidos" sheetId="11" r:id="rId11"/>
+    <sheet name="sangrado_mucosas" sheetId="12" r:id="rId12"/>
+    <sheet name="hemorragia" sheetId="13" r:id="rId13"/>
+    <sheet name="shock" sheetId="14" r:id="rId14"/>
+    <sheet name="letargia" sheetId="15" r:id="rId15"/>
+    <sheet name="irritabilidad" sheetId="16" r:id="rId16"/>
     <sheet name="hepatomegalia" sheetId="17" r:id="rId17"/>
+    <sheet name="clase" sheetId="18" r:id="rId18"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="34">
   <si>
     <t>sexo</t>
   </si>
@@ -38,7 +39,7 @@
     <t>No Dengue</t>
   </si>
   <si>
-    <t>NNo signos Alerta</t>
+    <t>No signos Alerta</t>
   </si>
   <si>
     <t>Signos Alerta</t>
@@ -68,24 +69,33 @@
     <t>No</t>
   </si>
   <si>
+    <t>vomitos</t>
+  </si>
+  <si>
+    <t>Persistente</t>
+  </si>
+  <si>
     <t>rash</t>
   </si>
   <si>
-    <t>vomitos</t>
-  </si>
-  <si>
-    <t>NO</t>
-  </si>
-  <si>
-    <t>Persistente</t>
-  </si>
-  <si>
     <t>mialgias</t>
   </si>
   <si>
     <t>artralgias</t>
   </si>
   <si>
+    <t>prueba_torniquete</t>
+  </si>
+  <si>
+    <t>Positiva</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Negativa</t>
+  </si>
+  <si>
     <t>dolor_abdominal</t>
   </si>
   <si>
@@ -98,25 +108,31 @@
     <t>hemorragia</t>
   </si>
   <si>
+    <t>shock</t>
+  </si>
+  <si>
     <t>letargia</t>
   </si>
   <si>
     <t>irritabilidad</t>
   </si>
   <si>
-    <t>shock</t>
-  </si>
-  <si>
-    <t>prueba_torniquete</t>
-  </si>
-  <si>
-    <t>Positiva</t>
-  </si>
-  <si>
-    <t>Negativa</t>
-  </si>
-  <si>
     <t>hepatomegalia</t>
+  </si>
+  <si>
+    <t>clase</t>
+  </si>
+  <si>
+    <t>Dengue_NoGrave_NoSignos</t>
+  </si>
+  <si>
+    <t>No_Dengue</t>
+  </si>
+  <si>
+    <t>Dengue_Grave</t>
+  </si>
+  <si>
+    <t>Dengue_NoGrave_SignosAlarma</t>
   </si>
 </sst>
 </file>
@@ -546,7 +562,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -566,16 +582,16 @@
         <v>11</v>
       </c>
       <c r="B2">
-        <v>5680</v>
+        <v>3638</v>
       </c>
       <c r="C2">
-        <v>1785</v>
+        <v>1799</v>
       </c>
       <c r="D2">
-        <v>658</v>
+        <v>671</v>
       </c>
       <c r="E2">
-        <v>251</v>
+        <v>273</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -583,16 +599,16 @@
         <v>10</v>
       </c>
       <c r="B3">
-        <v>302</v>
+        <v>2344</v>
       </c>
       <c r="C3">
-        <v>195</v>
+        <v>181</v>
       </c>
       <c r="D3">
-        <v>384</v>
+        <v>371</v>
       </c>
       <c r="E3">
-        <v>745</v>
+        <v>723</v>
       </c>
     </row>
   </sheetData>
@@ -610,7 +626,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -630,16 +646,16 @@
         <v>11</v>
       </c>
       <c r="B2">
-        <v>5918</v>
+        <v>5680</v>
       </c>
       <c r="C2">
-        <v>1867</v>
+        <v>1785</v>
       </c>
       <c r="D2">
-        <v>887</v>
+        <v>658</v>
       </c>
       <c r="E2">
-        <v>197</v>
+        <v>251</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -647,16 +663,16 @@
         <v>10</v>
       </c>
       <c r="B3">
-        <v>64</v>
+        <v>302</v>
       </c>
       <c r="C3">
-        <v>113</v>
+        <v>195</v>
       </c>
       <c r="D3">
-        <v>155</v>
+        <v>384</v>
       </c>
       <c r="E3">
-        <v>799</v>
+        <v>745</v>
       </c>
     </row>
   </sheetData>
@@ -674,7 +690,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -694,13 +710,13 @@
         <v>11</v>
       </c>
       <c r="B2">
-        <v>4987</v>
+        <v>5918</v>
       </c>
       <c r="C2">
-        <v>1980</v>
+        <v>1867</v>
       </c>
       <c r="D2">
-        <v>1042</v>
+        <v>887</v>
       </c>
       <c r="E2">
         <v>197</v>
@@ -711,13 +727,13 @@
         <v>10</v>
       </c>
       <c r="B3">
-        <v>995</v>
+        <v>64</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>113</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>155</v>
       </c>
       <c r="E3">
         <v>799</v>
@@ -738,7 +754,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -758,16 +774,16 @@
         <v>11</v>
       </c>
       <c r="B2">
-        <v>5658</v>
+        <v>4987</v>
       </c>
       <c r="C2">
-        <v>1797</v>
+        <v>1980</v>
       </c>
       <c r="D2">
-        <v>652</v>
+        <v>1042</v>
       </c>
       <c r="E2">
-        <v>307</v>
+        <v>197</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -775,16 +791,16 @@
         <v>10</v>
       </c>
       <c r="B3">
-        <v>324</v>
+        <v>995</v>
       </c>
       <c r="C3">
-        <v>183</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>390</v>
+        <v>0</v>
       </c>
       <c r="E3">
-        <v>689</v>
+        <v>799</v>
       </c>
     </row>
   </sheetData>
@@ -802,7 +818,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -822,16 +838,16 @@
         <v>11</v>
       </c>
       <c r="B2">
-        <v>5682</v>
+        <v>5521</v>
       </c>
       <c r="C2">
-        <v>1969</v>
+        <v>1980</v>
       </c>
       <c r="D2">
-        <v>1011</v>
+        <v>1042</v>
       </c>
       <c r="E2">
-        <v>923</v>
+        <v>592</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -839,16 +855,16 @@
         <v>10</v>
       </c>
       <c r="B3">
-        <v>300</v>
+        <v>461</v>
       </c>
       <c r="C3">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="E3">
-        <v>73</v>
+        <v>404</v>
       </c>
     </row>
   </sheetData>
@@ -866,7 +882,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -886,16 +902,16 @@
         <v>11</v>
       </c>
       <c r="B2">
-        <v>5521</v>
+        <v>5658</v>
       </c>
       <c r="C2">
-        <v>1980</v>
+        <v>1797</v>
       </c>
       <c r="D2">
-        <v>1042</v>
+        <v>652</v>
       </c>
       <c r="E2">
-        <v>592</v>
+        <v>307</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -903,16 +919,16 @@
         <v>10</v>
       </c>
       <c r="B3">
-        <v>461</v>
+        <v>324</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>183</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>390</v>
       </c>
       <c r="E3">
-        <v>404</v>
+        <v>689</v>
       </c>
     </row>
   </sheetData>
@@ -922,7 +938,7 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -930,7 +946,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -947,50 +963,36 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="B2">
-        <v>194</v>
+        <v>5682</v>
       </c>
       <c r="C2">
-        <v>421</v>
+        <v>1969</v>
       </c>
       <c r="D2">
-        <v>222</v>
+        <v>1011</v>
       </c>
       <c r="E2">
-        <v>741</v>
+        <v>923</v>
       </c>
     </row>
     <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
       <c r="B3">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="E3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4">
-        <v>721</v>
-      </c>
-      <c r="C4">
-        <v>1062</v>
-      </c>
-      <c r="D4">
-        <v>558</v>
-      </c>
-      <c r="E4">
-        <v>11</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1062,6 +1064,104 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2">
+        <v>10000</v>
+      </c>
+      <c r="C2">
+        <v>10000</v>
+      </c>
+      <c r="D2">
+        <v>10000</v>
+      </c>
+      <c r="E2">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3">
+        <v>10000</v>
+      </c>
+      <c r="C3">
+        <v>10000</v>
+      </c>
+      <c r="D3">
+        <v>10000</v>
+      </c>
+      <c r="E3">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4">
+        <v>10000</v>
+      </c>
+      <c r="C4">
+        <v>10000</v>
+      </c>
+      <c r="D4">
+        <v>10000</v>
+      </c>
+      <c r="E4">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5">
+        <v>10000</v>
+      </c>
+      <c r="C5">
+        <v>10000</v>
+      </c>
+      <c r="D5">
+        <v>10000</v>
+      </c>
+      <c r="E5">
+        <v>10000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E6"/>
@@ -1358,6 +1458,87 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2">
+        <v>3670</v>
+      </c>
+      <c r="C2">
+        <v>1697</v>
+      </c>
+      <c r="D2">
+        <v>625</v>
+      </c>
+      <c r="E2">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <v>1835</v>
+      </c>
+      <c r="C3">
+        <v>103</v>
+      </c>
+      <c r="D3">
+        <v>35</v>
+      </c>
+      <c r="E3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4">
+        <v>477</v>
+      </c>
+      <c r="C4">
+        <v>180</v>
+      </c>
+      <c r="D4">
+        <v>382</v>
+      </c>
+      <c r="E4">
+        <v>745</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1366,7 +1547,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -1413,104 +1594,6 @@
       </c>
       <c r="E3">
         <v>531</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>1697</v>
-      </c>
-      <c r="D2">
-        <v>625</v>
-      </c>
-      <c r="E2">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3">
-        <v>1835</v>
-      </c>
-      <c r="C3">
-        <v>103</v>
-      </c>
-      <c r="D3">
-        <v>35</v>
-      </c>
-      <c r="E3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4">
-        <v>3670</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5">
-        <v>477</v>
-      </c>
-      <c r="C5">
-        <v>180</v>
-      </c>
-      <c r="D5">
-        <v>382</v>
-      </c>
-      <c r="E5">
-        <v>745</v>
       </c>
     </row>
   </sheetData>
@@ -1528,7 +1611,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -1592,7 +1675,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -1648,7 +1731,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1656,7 +1739,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -1673,36 +1756,53 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B2">
-        <v>3638</v>
+        <v>194</v>
       </c>
       <c r="C2">
-        <v>1799</v>
+        <v>421</v>
       </c>
       <c r="D2">
-        <v>671</v>
+        <v>222</v>
       </c>
       <c r="E2">
-        <v>273</v>
+        <v>741</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="B3">
-        <v>2344</v>
+        <v>5067</v>
       </c>
       <c r="C3">
-        <v>181</v>
+        <v>497</v>
       </c>
       <c r="D3">
-        <v>371</v>
+        <v>262</v>
       </c>
       <c r="E3">
-        <v>723</v>
+        <v>244</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4">
+        <v>721</v>
+      </c>
+      <c r="C4">
+        <v>1062</v>
+      </c>
+      <c r="D4">
+        <v>558</v>
+      </c>
+      <c r="E4">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mejoras en graficas y excel-2.0
</commit_message>
<xml_diff>
--- a/GRAFICAS/estadisticas.xlsx
+++ b/GRAFICAS/estadisticas.xlsx
@@ -24,14 +24,13 @@
     <sheet name="letargia" sheetId="15" r:id="rId15"/>
     <sheet name="irritabilidad" sheetId="16" r:id="rId16"/>
     <sheet name="hepatomegalia" sheetId="17" r:id="rId17"/>
-    <sheet name="clase" sheetId="18" r:id="rId18"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="29">
   <si>
     <t>sexo</t>
   </si>
@@ -118,21 +117,6 @@
   </si>
   <si>
     <t>hepatomegalia</t>
-  </si>
-  <si>
-    <t>clase</t>
-  </si>
-  <si>
-    <t>Dengue_NoGrave_NoSignos</t>
-  </si>
-  <si>
-    <t>No_Dengue</t>
-  </si>
-  <si>
-    <t>Dengue_Grave</t>
-  </si>
-  <si>
-    <t>Dengue_NoGrave_SignosAlarma</t>
   </si>
 </sst>
 </file>
@@ -1064,104 +1048,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B2">
-        <v>10000</v>
-      </c>
-      <c r="C2">
-        <v>10000</v>
-      </c>
-      <c r="D2">
-        <v>10000</v>
-      </c>
-      <c r="E2">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3">
-        <v>10000</v>
-      </c>
-      <c r="C3">
-        <v>10000</v>
-      </c>
-      <c r="D3">
-        <v>10000</v>
-      </c>
-      <c r="E3">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B4">
-        <v>10000</v>
-      </c>
-      <c r="C4">
-        <v>10000</v>
-      </c>
-      <c r="D4">
-        <v>10000</v>
-      </c>
-      <c r="E4">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5">
-        <v>10000</v>
-      </c>
-      <c r="C5">
-        <v>10000</v>
-      </c>
-      <c r="D5">
-        <v>10000</v>
-      </c>
-      <c r="E5">
-        <v>10000</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E6"/>

</xml_diff>